<commit_message>
Structured the repository by renaming the Jupyter notebook and formatting / commenting the code.
</commit_message>
<xml_diff>
--- a/transformed_data/cartel_networks/cartel_data_with_centrality_measures.xlsx
+++ b/transformed_data/cartel_networks/cartel_data_with_centrality_measures.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>key_iustin_long</t>
+          <t>key_invented</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>number_of_cartel_firms</t>
+          <t>number_cartel_firms</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -496,7 +496,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>cartel_classification</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -657,7 +657,7 @@
         <v>0.006032432325946102</v>
       </c>
       <c r="Z2" t="n">
-        <v>27.39682539682539</v>
+        <v>27.3968253968254</v>
       </c>
       <c r="AA2" t="n">
         <v>5</v>
@@ -750,7 +750,7 @@
         <v>0.003884517316208416</v>
       </c>
       <c r="Z3" t="n">
-        <v>26.67619047619047</v>
+        <v>26.67619047619048</v>
       </c>
       <c r="AA3" t="n">
         <v>3</v>
@@ -843,7 +843,7 @@
         <v>0.00156945221192517</v>
       </c>
       <c r="Z4" t="n">
-        <v>21.63015873015872</v>
+        <v>21.63015873015873</v>
       </c>
       <c r="AA4" t="n">
         <v>1</v>
@@ -936,7 +936,7 @@
         <v>0.006562735571552793</v>
       </c>
       <c r="Z5" t="n">
-        <v>29.21071428571428</v>
+        <v>29.21071428571429</v>
       </c>
       <c r="AA5" t="n">
         <v>5</v>
@@ -1122,7 +1122,7 @@
         <v>0.002804333319768834</v>
       </c>
       <c r="Z7" t="n">
-        <v>24.29682539682539</v>
+        <v>24.2968253968254</v>
       </c>
       <c r="AA7" t="n">
         <v>2</v>
@@ -1581,7 +1581,7 @@
         <v>0.001656722492272191</v>
       </c>
       <c r="Z12" t="n">
-        <v>16.85241702741701</v>
+        <v>16.85241702741702</v>
       </c>
       <c r="AA12" t="n">
         <v>1</v>
@@ -1672,7 +1672,7 @@
         <v>0.001656722492272191</v>
       </c>
       <c r="Z13" t="n">
-        <v>16.85241702741701</v>
+        <v>16.85241702741702</v>
       </c>
       <c r="AA13" t="n">
         <v>1</v>
@@ -1763,7 +1763,7 @@
         <v>0.006032432325946102</v>
       </c>
       <c r="Z14" t="n">
-        <v>27.39682539682539</v>
+        <v>27.3968253968254</v>
       </c>
       <c r="AA14" t="n">
         <v>5</v>
@@ -2670,7 +2670,7 @@
         <v>0.003224627315347335</v>
       </c>
       <c r="S24" t="n">
-        <v>19.32817460317458</v>
+        <v>19.32817460317459</v>
       </c>
       <c r="T24" t="n">
         <v>2</v>
@@ -2691,7 +2691,7 @@
         <v>0.004049323846751346</v>
       </c>
       <c r="Z24" t="n">
-        <v>24.8702380952381</v>
+        <v>24.87023809523809</v>
       </c>
       <c r="AA24" t="n">
         <v>3</v>
@@ -2761,7 +2761,7 @@
         <v>0.003224627315347335</v>
       </c>
       <c r="S25" t="n">
-        <v>19.32817460317458</v>
+        <v>19.32817460317459</v>
       </c>
       <c r="T25" t="n">
         <v>2</v>
@@ -3036,7 +3036,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S28" t="n">
-        <v>6.833333333333332</v>
+        <v>6.833333333333333</v>
       </c>
       <c r="T28" t="n">
         <v>5</v>
@@ -3129,7 +3129,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S29" t="n">
-        <v>6.833333333333332</v>
+        <v>6.833333333333333</v>
       </c>
       <c r="T29" t="n">
         <v>5</v>
@@ -3222,7 +3222,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S30" t="n">
-        <v>6.833333333333332</v>
+        <v>6.833333333333333</v>
       </c>
       <c r="T30" t="n">
         <v>5</v>
@@ -3315,7 +3315,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S31" t="n">
-        <v>6.833333333333332</v>
+        <v>6.833333333333333</v>
       </c>
       <c r="T31" t="n">
         <v>5</v>
@@ -3408,7 +3408,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S32" t="n">
-        <v>6.833333333333332</v>
+        <v>6.833333333333333</v>
       </c>
       <c r="T32" t="n">
         <v>5</v>
@@ -3429,7 +3429,7 @@
         <v>0.001952215469372171</v>
       </c>
       <c r="Z32" t="n">
-        <v>4.333333333333334</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="AA32" t="n">
         <v>1</v>
@@ -4320,7 +4320,7 @@
         <v>0.00431334221512761</v>
       </c>
       <c r="S42" t="n">
-        <v>7.666666666666666</v>
+        <v>7.666666666666665</v>
       </c>
       <c r="T42" t="n">
         <v>4</v>
@@ -4413,7 +4413,7 @@
         <v>0.00431334221512761</v>
       </c>
       <c r="S43" t="n">
-        <v>7.666666666666666</v>
+        <v>7.666666666666665</v>
       </c>
       <c r="T43" t="n">
         <v>4</v>
@@ -4506,7 +4506,7 @@
         <v>0.00431334221512761</v>
       </c>
       <c r="S44" t="n">
-        <v>7.666666666666666</v>
+        <v>7.666666666666665</v>
       </c>
       <c r="T44" t="n">
         <v>4</v>
@@ -4599,7 +4599,7 @@
         <v>0.00431334221512761</v>
       </c>
       <c r="S45" t="n">
-        <v>7.666666666666666</v>
+        <v>7.666666666666665</v>
       </c>
       <c r="T45" t="n">
         <v>4</v>
@@ -4783,7 +4783,7 @@
         <v>0.008783637448984945</v>
       </c>
       <c r="S47" t="n">
-        <v>10.33333333333334</v>
+        <v>10.33333333333333</v>
       </c>
       <c r="T47" t="n">
         <v>8</v>
@@ -4876,7 +4876,7 @@
         <v>0.008783637448984945</v>
       </c>
       <c r="S48" t="n">
-        <v>10.33333333333334</v>
+        <v>10.33333333333333</v>
       </c>
       <c r="T48" t="n">
         <v>8</v>
@@ -4969,7 +4969,7 @@
         <v>0.008783637448984945</v>
       </c>
       <c r="S49" t="n">
-        <v>10.33333333333334</v>
+        <v>10.33333333333333</v>
       </c>
       <c r="T49" t="n">
         <v>8</v>
@@ -5062,7 +5062,7 @@
         <v>0.008783637448984945</v>
       </c>
       <c r="S50" t="n">
-        <v>10.33333333333334</v>
+        <v>10.33333333333333</v>
       </c>
       <c r="T50" t="n">
         <v>8</v>
@@ -5155,7 +5155,7 @@
         <v>0.008783637448984945</v>
       </c>
       <c r="S51" t="n">
-        <v>10.33333333333334</v>
+        <v>10.33333333333333</v>
       </c>
       <c r="T51" t="n">
         <v>8</v>
@@ -5248,7 +5248,7 @@
         <v>0.008783637448984945</v>
       </c>
       <c r="S52" t="n">
-        <v>10.33333333333334</v>
+        <v>10.33333333333333</v>
       </c>
       <c r="T52" t="n">
         <v>8</v>
@@ -5341,7 +5341,7 @@
         <v>0.008783637448984945</v>
       </c>
       <c r="S53" t="n">
-        <v>10.33333333333334</v>
+        <v>10.33333333333333</v>
       </c>
       <c r="T53" t="n">
         <v>8</v>
@@ -5434,7 +5434,7 @@
         <v>0.008783637448984945</v>
       </c>
       <c r="S54" t="n">
-        <v>10.33333333333334</v>
+        <v>10.33333333333333</v>
       </c>
       <c r="T54" t="n">
         <v>8</v>
@@ -5527,7 +5527,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S55" t="n">
-        <v>6.833333333333333</v>
+        <v>6.833333333333332</v>
       </c>
       <c r="T55" t="n">
         <v>5</v>
@@ -5620,7 +5620,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S56" t="n">
-        <v>6.833333333333333</v>
+        <v>6.833333333333332</v>
       </c>
       <c r="T56" t="n">
         <v>5</v>
@@ -5641,7 +5641,7 @@
         <v>0.001952215469372171</v>
       </c>
       <c r="Z56" t="n">
-        <v>4.333333333333334</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="AA56" t="n">
         <v>1</v>
@@ -5713,7 +5713,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S57" t="n">
-        <v>6.833333333333333</v>
+        <v>6.833333333333332</v>
       </c>
       <c r="T57" t="n">
         <v>5</v>
@@ -5734,7 +5734,7 @@
         <v>0.001952215469372171</v>
       </c>
       <c r="Z57" t="n">
-        <v>4.333333333333334</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="AA57" t="n">
         <v>1</v>
@@ -5806,7 +5806,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S58" t="n">
-        <v>6.833333333333333</v>
+        <v>6.833333333333332</v>
       </c>
       <c r="T58" t="n">
         <v>5</v>
@@ -5827,7 +5827,7 @@
         <v>0.001952215469372171</v>
       </c>
       <c r="Z58" t="n">
-        <v>4.333333333333334</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="AA58" t="n">
         <v>1</v>
@@ -5899,7 +5899,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S59" t="n">
-        <v>6.833333333333333</v>
+        <v>6.833333333333332</v>
       </c>
       <c r="T59" t="n">
         <v>5</v>
@@ -5920,7 +5920,7 @@
         <v>0.001952215469372171</v>
       </c>
       <c r="Z59" t="n">
-        <v>4.333333333333334</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="AA59" t="n">
         <v>1</v>
@@ -6013,7 +6013,7 @@
         <v>0.001762389124862823</v>
       </c>
       <c r="Z60" t="n">
-        <v>5.916666666666666</v>
+        <v>5.916666666666667</v>
       </c>
       <c r="AA60" t="n">
         <v>1</v>
@@ -6199,7 +6199,7 @@
         <v>0.00297776980412998</v>
       </c>
       <c r="Z62" t="n">
-        <v>7.583333333333333</v>
+        <v>7.583333333333334</v>
       </c>
       <c r="AA62" t="n">
         <v>2</v>
@@ -6385,7 +6385,7 @@
         <v>0.001762389124862823</v>
       </c>
       <c r="Z64" t="n">
-        <v>5.916666666666666</v>
+        <v>5.916666666666667</v>
       </c>
       <c r="AA64" t="n">
         <v>1</v>
@@ -6664,7 +6664,7 @@
         <v>0.002867355746022141</v>
       </c>
       <c r="Z67" t="n">
-        <v>18.36785714285714</v>
+        <v>18.36785714285713</v>
       </c>
       <c r="AA67" t="n">
         <v>2</v>
@@ -7288,7 +7288,7 @@
         <v>0.004090150686838246</v>
       </c>
       <c r="S74" t="n">
-        <v>21.64999999999999</v>
+        <v>21.64999999999998</v>
       </c>
       <c r="T74" t="n">
         <v>3</v>
@@ -7309,7 +7309,7 @@
         <v>0.002867355746022141</v>
       </c>
       <c r="Z74" t="n">
-        <v>18.36785714285714</v>
+        <v>18.36785714285713</v>
       </c>
       <c r="AA74" t="n">
         <v>2</v>
@@ -7381,7 +7381,7 @@
         <v>0.004090150686838246</v>
       </c>
       <c r="S75" t="n">
-        <v>21.64999999999999</v>
+        <v>21.64999999999998</v>
       </c>
       <c r="T75" t="n">
         <v>3</v>
@@ -7402,7 +7402,7 @@
         <v>0.004174246710644446</v>
       </c>
       <c r="Z75" t="n">
-        <v>22.23571428571428</v>
+        <v>22.23571428571429</v>
       </c>
       <c r="AA75" t="n">
         <v>3</v>
@@ -7474,7 +7474,7 @@
         <v>0.004090150686838246</v>
       </c>
       <c r="S76" t="n">
-        <v>21.64999999999999</v>
+        <v>21.64999999999998</v>
       </c>
       <c r="T76" t="n">
         <v>3</v>
@@ -7495,7 +7495,7 @@
         <v>0.002815046164461936</v>
       </c>
       <c r="Z76" t="n">
-        <v>22.32738095238096</v>
+        <v>22.32738095238095</v>
       </c>
       <c r="AA76" t="n">
         <v>2</v>
@@ -7939,7 +7939,7 @@
         <v>0.003756245390724891</v>
       </c>
       <c r="S81" t="n">
-        <v>5.166666666666667</v>
+        <v>5.166666666666666</v>
       </c>
       <c r="T81" t="n">
         <v>2</v>
@@ -8032,7 +8032,7 @@
         <v>0.003756245390724891</v>
       </c>
       <c r="S82" t="n">
-        <v>5.166666666666667</v>
+        <v>5.166666666666666</v>
       </c>
       <c r="T82" t="n">
         <v>2</v>
@@ -8214,7 +8214,7 @@
         <v>0.01367145808664726</v>
       </c>
       <c r="S84" t="n">
-        <v>28.68095238095236</v>
+        <v>28.68095238095235</v>
       </c>
       <c r="T84" t="n">
         <v>10</v>
@@ -8235,7 +8235,7 @@
         <v>0.004049323846751346</v>
       </c>
       <c r="Z84" t="n">
-        <v>24.8702380952381</v>
+        <v>24.87023809523809</v>
       </c>
       <c r="AA84" t="n">
         <v>3</v>
@@ -8305,7 +8305,7 @@
         <v>0.01367145808664726</v>
       </c>
       <c r="S85" t="n">
-        <v>28.68095238095236</v>
+        <v>28.68095238095235</v>
       </c>
       <c r="T85" t="n">
         <v>10</v>
@@ -8396,7 +8396,7 @@
         <v>0.01367145808664726</v>
       </c>
       <c r="S86" t="n">
-        <v>28.68095238095236</v>
+        <v>28.68095238095235</v>
       </c>
       <c r="T86" t="n">
         <v>10</v>
@@ -8417,7 +8417,7 @@
         <v>0.003040916061606044</v>
       </c>
       <c r="Z86" t="n">
-        <v>21.25357142857143</v>
+        <v>21.25357142857142</v>
       </c>
       <c r="AA86" t="n">
         <v>2</v>
@@ -8487,7 +8487,7 @@
         <v>0.01367145808664726</v>
       </c>
       <c r="S87" t="n">
-        <v>28.68095238095236</v>
+        <v>28.68095238095235</v>
       </c>
       <c r="T87" t="n">
         <v>10</v>
@@ -8508,7 +8508,7 @@
         <v>0.003884517316208416</v>
       </c>
       <c r="Z87" t="n">
-        <v>26.67619047619047</v>
+        <v>26.67619047619048</v>
       </c>
       <c r="AA87" t="n">
         <v>3</v>
@@ -8578,7 +8578,7 @@
         <v>0.01367145808664726</v>
       </c>
       <c r="S88" t="n">
-        <v>28.68095238095236</v>
+        <v>28.68095238095235</v>
       </c>
       <c r="T88" t="n">
         <v>10</v>
@@ -8669,7 +8669,7 @@
         <v>0.01367145808664726</v>
       </c>
       <c r="S89" t="n">
-        <v>28.68095238095236</v>
+        <v>28.68095238095235</v>
       </c>
       <c r="T89" t="n">
         <v>10</v>
@@ -8760,7 +8760,7 @@
         <v>0.01367145808664726</v>
       </c>
       <c r="S90" t="n">
-        <v>28.68095238095236</v>
+        <v>28.68095238095235</v>
       </c>
       <c r="T90" t="n">
         <v>10</v>
@@ -8851,7 +8851,7 @@
         <v>0.01367145808664726</v>
       </c>
       <c r="S91" t="n">
-        <v>28.68095238095236</v>
+        <v>28.68095238095235</v>
       </c>
       <c r="T91" t="n">
         <v>10</v>
@@ -8872,7 +8872,7 @@
         <v>0.001655839492786507</v>
       </c>
       <c r="Z91" t="n">
-        <v>20.1202380952381</v>
+        <v>20.12023809523809</v>
       </c>
       <c r="AA91" t="n">
         <v>1</v>
@@ -8942,7 +8942,7 @@
         <v>0.01367145808664726</v>
       </c>
       <c r="S92" t="n">
-        <v>28.68095238095236</v>
+        <v>28.68095238095235</v>
       </c>
       <c r="T92" t="n">
         <v>10</v>
@@ -9033,7 +9033,7 @@
         <v>0.01367145808664726</v>
       </c>
       <c r="S93" t="n">
-        <v>28.68095238095236</v>
+        <v>28.68095238095235</v>
       </c>
       <c r="T93" t="n">
         <v>10</v>
@@ -9054,7 +9054,7 @@
         <v>0.002815046164461936</v>
       </c>
       <c r="Z93" t="n">
-        <v>22.32738095238096</v>
+        <v>22.32738095238095</v>
       </c>
       <c r="AA93" t="n">
         <v>2</v>
@@ -9126,7 +9126,7 @@
         <v>0.003734692891254172</v>
       </c>
       <c r="S94" t="n">
-        <v>13.37002164502163</v>
+        <v>13.37002164502164</v>
       </c>
       <c r="T94" t="n">
         <v>2</v>
@@ -9219,7 +9219,7 @@
         <v>0.003734692891254172</v>
       </c>
       <c r="S95" t="n">
-        <v>13.37002164502163</v>
+        <v>13.37002164502164</v>
       </c>
       <c r="T95" t="n">
         <v>2</v>
@@ -9333,7 +9333,7 @@
         <v>0.001646067716759898</v>
       </c>
       <c r="Z96" t="n">
-        <v>17.40039682539681</v>
+        <v>17.40039682539682</v>
       </c>
       <c r="AA96" t="n">
         <v>1</v>
@@ -9426,7 +9426,7 @@
         <v>0.003884517316208416</v>
       </c>
       <c r="Z97" t="n">
-        <v>26.67619047619047</v>
+        <v>26.67619047619048</v>
       </c>
       <c r="AA97" t="n">
         <v>3</v>
@@ -9984,7 +9984,7 @@
         <v>0.00297776980412998</v>
       </c>
       <c r="Z103" t="n">
-        <v>7.583333333333333</v>
+        <v>7.583333333333334</v>
       </c>
       <c r="AA103" t="n">
         <v>2</v>
@@ -11001,7 +11001,7 @@
         <v>0.006032432325946102</v>
       </c>
       <c r="Z114" t="n">
-        <v>27.39682539682539</v>
+        <v>27.3968253968254</v>
       </c>
       <c r="AA114" t="n">
         <v>5</v>
@@ -11094,7 +11094,7 @@
         <v>0.0016180402480738</v>
       </c>
       <c r="Z115" t="n">
-        <v>16.81908369408368</v>
+        <v>16.81908369408369</v>
       </c>
       <c r="AA115" t="n">
         <v>1</v>
@@ -11648,7 +11648,7 @@
         <v>0.003040916061606044</v>
       </c>
       <c r="Z121" t="n">
-        <v>21.25357142857143</v>
+        <v>21.25357142857142</v>
       </c>
       <c r="AA121" t="n">
         <v>2</v>
@@ -11720,7 +11720,7 @@
         <v>0.008215477340849063</v>
       </c>
       <c r="S122" t="n">
-        <v>8.166666666666668</v>
+        <v>8.166666666666666</v>
       </c>
       <c r="T122" t="n">
         <v>6</v>
@@ -11813,7 +11813,7 @@
         <v>0.008215477340849063</v>
       </c>
       <c r="S123" t="n">
-        <v>8.166666666666668</v>
+        <v>8.166666666666666</v>
       </c>
       <c r="T123" t="n">
         <v>6</v>
@@ -11834,7 +11834,7 @@
         <v>0.002923329799450725</v>
       </c>
       <c r="Z123" t="n">
-        <v>5.666666666666666</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="AA123" t="n">
         <v>2</v>
@@ -11906,7 +11906,7 @@
         <v>0.008215477340849063</v>
       </c>
       <c r="S124" t="n">
-        <v>8.166666666666668</v>
+        <v>8.166666666666666</v>
       </c>
       <c r="T124" t="n">
         <v>6</v>
@@ -11927,7 +11927,7 @@
         <v>0.002923329799450725</v>
       </c>
       <c r="Z124" t="n">
-        <v>5.666666666666666</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="AA124" t="n">
         <v>2</v>
@@ -11999,7 +11999,7 @@
         <v>0.008215477340849063</v>
       </c>
       <c r="S125" t="n">
-        <v>8.166666666666668</v>
+        <v>8.166666666666666</v>
       </c>
       <c r="T125" t="n">
         <v>6</v>
@@ -12092,7 +12092,7 @@
         <v>0.008215477340849063</v>
       </c>
       <c r="S126" t="n">
-        <v>8.166666666666668</v>
+        <v>8.166666666666666</v>
       </c>
       <c r="T126" t="n">
         <v>6</v>
@@ -12185,7 +12185,7 @@
         <v>0.008215477340849063</v>
       </c>
       <c r="S127" t="n">
-        <v>8.166666666666668</v>
+        <v>8.166666666666666</v>
       </c>
       <c r="T127" t="n">
         <v>6</v>
@@ -12206,7 +12206,7 @@
         <v>0.002926723212164678</v>
       </c>
       <c r="Z127" t="n">
-        <v>5.916666666666666</v>
+        <v>5.916666666666667</v>
       </c>
       <c r="AA127" t="n">
         <v>2</v>
@@ -12460,7 +12460,7 @@
         <v>0.00297774247180845</v>
       </c>
       <c r="S130" t="n">
-        <v>4.733333333333333</v>
+        <v>4.733333333333334</v>
       </c>
       <c r="T130" t="n">
         <v>2</v>
@@ -12481,7 +12481,7 @@
         <v>0.002923329799450725</v>
       </c>
       <c r="Z130" t="n">
-        <v>5.666666666666666</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="AA130" t="n">
         <v>2</v>
@@ -12553,7 +12553,7 @@
         <v>0.00297774247180845</v>
       </c>
       <c r="S131" t="n">
-        <v>4.733333333333333</v>
+        <v>4.733333333333334</v>
       </c>
       <c r="T131" t="n">
         <v>2</v>
@@ -12574,7 +12574,7 @@
         <v>0.002923329799450725</v>
       </c>
       <c r="Z131" t="n">
-        <v>5.666666666666666</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="AA131" t="n">
         <v>2</v>
@@ -13845,7 +13845,7 @@
         <v>0.004851114696581942</v>
       </c>
       <c r="S145" t="n">
-        <v>18.52301587301586</v>
+        <v>18.52301587301585</v>
       </c>
       <c r="T145" t="n">
         <v>3</v>
@@ -13938,7 +13938,7 @@
         <v>0.004851114696581942</v>
       </c>
       <c r="S146" t="n">
-        <v>18.52301587301586</v>
+        <v>18.52301587301585</v>
       </c>
       <c r="T146" t="n">
         <v>3</v>
@@ -13959,7 +13959,7 @@
         <v>0.004174246710644446</v>
       </c>
       <c r="Z146" t="n">
-        <v>22.23571428571428</v>
+        <v>22.23571428571429</v>
       </c>
       <c r="AA146" t="n">
         <v>3</v>
@@ -14031,7 +14031,7 @@
         <v>0.004851114696581942</v>
       </c>
       <c r="S147" t="n">
-        <v>18.52301587301586</v>
+        <v>18.52301587301585</v>
       </c>
       <c r="T147" t="n">
         <v>3</v>
@@ -14122,7 +14122,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S148" t="n">
-        <v>25.58015873015871</v>
+        <v>25.5801587301587</v>
       </c>
       <c r="T148" t="n">
         <v>9</v>
@@ -14143,7 +14143,7 @@
         <v>0.001728302160475243</v>
       </c>
       <c r="Z148" t="n">
-        <v>18.30241702741703</v>
+        <v>18.30241702741702</v>
       </c>
       <c r="AA148" t="n">
         <v>1</v>
@@ -14213,7 +14213,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S149" t="n">
-        <v>25.58015873015871</v>
+        <v>25.5801587301587</v>
       </c>
       <c r="T149" t="n">
         <v>9</v>
@@ -14234,7 +14234,7 @@
         <v>0.001728302160475243</v>
       </c>
       <c r="Z149" t="n">
-        <v>18.30241702741703</v>
+        <v>18.30241702741702</v>
       </c>
       <c r="AA149" t="n">
         <v>1</v>
@@ -14304,7 +14304,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S150" t="n">
-        <v>25.58015873015871</v>
+        <v>25.5801587301587</v>
       </c>
       <c r="T150" t="n">
         <v>9</v>
@@ -14325,7 +14325,7 @@
         <v>0.001728302160475243</v>
       </c>
       <c r="Z150" t="n">
-        <v>18.30241702741703</v>
+        <v>18.30241702741702</v>
       </c>
       <c r="AA150" t="n">
         <v>1</v>
@@ -14395,7 +14395,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S151" t="n">
-        <v>25.58015873015871</v>
+        <v>25.5801587301587</v>
       </c>
       <c r="T151" t="n">
         <v>9</v>
@@ -14416,7 +14416,7 @@
         <v>0.001728302160475243</v>
       </c>
       <c r="Z151" t="n">
-        <v>18.30241702741703</v>
+        <v>18.30241702741702</v>
       </c>
       <c r="AA151" t="n">
         <v>1</v>
@@ -14486,7 +14486,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S152" t="n">
-        <v>25.58015873015871</v>
+        <v>25.5801587301587</v>
       </c>
       <c r="T152" t="n">
         <v>9</v>
@@ -14507,7 +14507,7 @@
         <v>0.001728302160475243</v>
       </c>
       <c r="Z152" t="n">
-        <v>18.30241702741703</v>
+        <v>18.30241702741702</v>
       </c>
       <c r="AA152" t="n">
         <v>1</v>
@@ -14577,7 +14577,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S153" t="n">
-        <v>25.58015873015871</v>
+        <v>25.5801587301587</v>
       </c>
       <c r="T153" t="n">
         <v>9</v>
@@ -14598,7 +14598,7 @@
         <v>0.001728302160475243</v>
       </c>
       <c r="Z153" t="n">
-        <v>18.30241702741703</v>
+        <v>18.30241702741702</v>
       </c>
       <c r="AA153" t="n">
         <v>1</v>
@@ -14668,7 +14668,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S154" t="n">
-        <v>25.58015873015871</v>
+        <v>25.5801587301587</v>
       </c>
       <c r="T154" t="n">
         <v>9</v>
@@ -14689,7 +14689,7 @@
         <v>0.001728302160475243</v>
       </c>
       <c r="Z154" t="n">
-        <v>18.30241702741703</v>
+        <v>18.30241702741702</v>
       </c>
       <c r="AA154" t="n">
         <v>1</v>
@@ -14759,7 +14759,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S155" t="n">
-        <v>25.58015873015871</v>
+        <v>25.5801587301587</v>
       </c>
       <c r="T155" t="n">
         <v>9</v>
@@ -14850,7 +14850,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S156" t="n">
-        <v>25.58015873015871</v>
+        <v>25.5801587301587</v>
       </c>
       <c r="T156" t="n">
         <v>9</v>
@@ -14871,7 +14871,7 @@
         <v>0.002804333319768834</v>
       </c>
       <c r="Z156" t="n">
-        <v>24.29682539682539</v>
+        <v>24.2968253968254</v>
       </c>
       <c r="AA156" t="n">
         <v>2</v>
@@ -14943,7 +14943,7 @@
         <v>0.007216240904336362</v>
       </c>
       <c r="S157" t="n">
-        <v>27.72976190476188</v>
+        <v>27.72976190476189</v>
       </c>
       <c r="T157" t="n">
         <v>6</v>
@@ -15036,7 +15036,7 @@
         <v>0.007216240904336362</v>
       </c>
       <c r="S158" t="n">
-        <v>27.72976190476188</v>
+        <v>27.72976190476189</v>
       </c>
       <c r="T158" t="n">
         <v>6</v>
@@ -15057,7 +15057,7 @@
         <v>0.004049323846751346</v>
       </c>
       <c r="Z158" t="n">
-        <v>24.8702380952381</v>
+        <v>24.87023809523809</v>
       </c>
       <c r="AA158" t="n">
         <v>3</v>
@@ -15129,7 +15129,7 @@
         <v>0.007216240904336362</v>
       </c>
       <c r="S159" t="n">
-        <v>27.72976190476188</v>
+        <v>27.72976190476189</v>
       </c>
       <c r="T159" t="n">
         <v>6</v>
@@ -15150,7 +15150,7 @@
         <v>0.006032432325946102</v>
       </c>
       <c r="Z159" t="n">
-        <v>27.39682539682539</v>
+        <v>27.3968253968254</v>
       </c>
       <c r="AA159" t="n">
         <v>5</v>
@@ -15222,7 +15222,7 @@
         <v>0.007216240904336362</v>
       </c>
       <c r="S160" t="n">
-        <v>27.72976190476188</v>
+        <v>27.72976190476189</v>
       </c>
       <c r="T160" t="n">
         <v>6</v>
@@ -15315,7 +15315,7 @@
         <v>0.007216240904336362</v>
       </c>
       <c r="S161" t="n">
-        <v>27.72976190476188</v>
+        <v>27.72976190476189</v>
       </c>
       <c r="T161" t="n">
         <v>6</v>
@@ -15408,7 +15408,7 @@
         <v>0.007216240904336362</v>
       </c>
       <c r="S162" t="n">
-        <v>27.72976190476188</v>
+        <v>27.72976190476189</v>
       </c>
       <c r="T162" t="n">
         <v>6</v>
@@ -15615,7 +15615,7 @@
         <v>0.006032432325946102</v>
       </c>
       <c r="Z164" t="n">
-        <v>27.39682539682539</v>
+        <v>27.3968253968254</v>
       </c>
       <c r="AA164" t="n">
         <v>5</v>
@@ -15871,7 +15871,7 @@
         <v>0.001608707494018752</v>
       </c>
       <c r="S167" t="n">
-        <v>21.05396825396824</v>
+        <v>21.05396825396825</v>
       </c>
       <c r="T167" t="n">
         <v>1</v>
@@ -15892,7 +15892,7 @@
         <v>0.006562735571552793</v>
       </c>
       <c r="Z167" t="n">
-        <v>29.21071428571428</v>
+        <v>29.21071428571429</v>
       </c>
       <c r="AA167" t="n">
         <v>5</v>
@@ -17742,7 +17742,7 @@
         <v>0.001913327899506806</v>
       </c>
       <c r="Z187" t="n">
-        <v>14.57150072150071</v>
+        <v>14.57150072150072</v>
       </c>
       <c r="AA187" t="n">
         <v>1</v>
@@ -17835,7 +17835,7 @@
         <v>0.003184124331344304</v>
       </c>
       <c r="Z188" t="n">
-        <v>20.72698412698412</v>
+        <v>20.72698412698413</v>
       </c>
       <c r="AA188" t="n">
         <v>2</v>
@@ -18573,7 +18573,7 @@
         <v>0.001701332547968635</v>
       </c>
       <c r="Z196" t="n">
-        <v>18.31031746031745</v>
+        <v>18.31031746031746</v>
       </c>
       <c r="AA196" t="n">
         <v>1</v>
@@ -18852,7 +18852,7 @@
         <v>0.006562735571552793</v>
       </c>
       <c r="Z199" t="n">
-        <v>29.21071428571428</v>
+        <v>29.21071428571429</v>
       </c>
       <c r="AA199" t="n">
         <v>5</v>
@@ -19017,7 +19017,7 @@
         <v>0.003570263981185514</v>
       </c>
       <c r="S201" t="n">
-        <v>16.02741702741702</v>
+        <v>16.02741702741701</v>
       </c>
       <c r="T201" t="n">
         <v>2</v>
@@ -19110,7 +19110,7 @@
         <v>0.003570263981185514</v>
       </c>
       <c r="S202" t="n">
-        <v>16.02741702741702</v>
+        <v>16.02741702741701</v>
       </c>
       <c r="T202" t="n">
         <v>2</v>
@@ -19203,7 +19203,7 @@
         <v>0.004689905761255771</v>
       </c>
       <c r="S203" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
       <c r="T203" t="n">
         <v>3</v>
@@ -19296,7 +19296,7 @@
         <v>0.004689905761255771</v>
       </c>
       <c r="S204" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
       <c r="T204" t="n">
         <v>3</v>
@@ -19389,7 +19389,7 @@
         <v>0.004689905761255771</v>
       </c>
       <c r="S205" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
       <c r="T205" t="n">
         <v>3</v>
@@ -19503,7 +19503,7 @@
         <v>0.001764217484469077</v>
       </c>
       <c r="Z206" t="n">
-        <v>19.06031746031745</v>
+        <v>19.06031746031746</v>
       </c>
       <c r="AA206" t="n">
         <v>1</v>
@@ -19596,7 +19596,7 @@
         <v>0.001764217484469077</v>
       </c>
       <c r="Z207" t="n">
-        <v>19.06031746031745</v>
+        <v>19.06031746031746</v>
       </c>
       <c r="AA207" t="n">
         <v>1</v>
@@ -19689,7 +19689,7 @@
         <v>0.003184124331344304</v>
       </c>
       <c r="Z208" t="n">
-        <v>20.72698412698412</v>
+        <v>20.72698412698413</v>
       </c>
       <c r="AA208" t="n">
         <v>2</v>
@@ -19782,7 +19782,7 @@
         <v>0.001764217484469077</v>
       </c>
       <c r="Z209" t="n">
-        <v>19.06031746031745</v>
+        <v>19.06031746031746</v>
       </c>
       <c r="AA209" t="n">
         <v>1</v>
@@ -19875,7 +19875,7 @@
         <v>0.006562735571552793</v>
       </c>
       <c r="Z210" t="n">
-        <v>29.21071428571428</v>
+        <v>29.21071428571429</v>
       </c>
       <c r="AA210" t="n">
         <v>5</v>
@@ -19968,7 +19968,7 @@
         <v>0.001764217484469077</v>
       </c>
       <c r="Z211" t="n">
-        <v>19.06031746031745</v>
+        <v>19.06031746031746</v>
       </c>
       <c r="AA211" t="n">
         <v>1</v>
@@ -20061,7 +20061,7 @@
         <v>0.001764217484469077</v>
       </c>
       <c r="Z212" t="n">
-        <v>19.06031746031745</v>
+        <v>19.06031746031746</v>
       </c>
       <c r="AA212" t="n">
         <v>1</v>
@@ -20154,7 +20154,7 @@
         <v>0.001764217484469077</v>
       </c>
       <c r="Z213" t="n">
-        <v>19.06031746031745</v>
+        <v>19.06031746031746</v>
       </c>
       <c r="AA213" t="n">
         <v>1</v>
@@ -20778,7 +20778,7 @@
         <v>0.003480727871408069</v>
       </c>
       <c r="S220" t="n">
-        <v>4.333333333333333</v>
+        <v>4.333333333333334</v>
       </c>
       <c r="T220" t="n">
         <v>2</v>
@@ -20871,7 +20871,7 @@
         <v>0.003480727871408069</v>
       </c>
       <c r="S221" t="n">
-        <v>4.333333333333333</v>
+        <v>4.333333333333334</v>
       </c>
       <c r="T221" t="n">
         <v>2</v>
@@ -20983,7 +20983,7 @@
         <v>0.001890394166277293</v>
       </c>
       <c r="Z222" t="n">
-        <v>7.366666666666667</v>
+        <v>7.366666666666666</v>
       </c>
       <c r="AA222" t="n">
         <v>1</v>
@@ -21074,7 +21074,7 @@
         <v>0.001890394166277293</v>
       </c>
       <c r="Z223" t="n">
-        <v>7.366666666666667</v>
+        <v>7.366666666666666</v>
       </c>
       <c r="AA223" t="n">
         <v>1</v>
@@ -21165,7 +21165,7 @@
         <v>0.001890394166277293</v>
       </c>
       <c r="Z224" t="n">
-        <v>7.366666666666667</v>
+        <v>7.366666666666666</v>
       </c>
       <c r="AA224" t="n">
         <v>1</v>
@@ -21256,7 +21256,7 @@
         <v>0.001890394166277293</v>
       </c>
       <c r="Z225" t="n">
-        <v>7.366666666666667</v>
+        <v>7.366666666666666</v>
       </c>
       <c r="AA225" t="n">
         <v>1</v>
@@ -21347,7 +21347,7 @@
         <v>0.001890394166277293</v>
       </c>
       <c r="Z226" t="n">
-        <v>7.366666666666667</v>
+        <v>7.366666666666666</v>
       </c>
       <c r="AA226" t="n">
         <v>1</v>
@@ -21438,7 +21438,7 @@
         <v>0.001890394166277293</v>
       </c>
       <c r="Z227" t="n">
-        <v>7.366666666666668</v>
+        <v>7.366666666666666</v>
       </c>
       <c r="AA227" t="n">
         <v>1</v>
@@ -24024,7 +24024,7 @@
         <v>0.001905724359327946</v>
       </c>
       <c r="Z255" t="n">
-        <v>7.033333333333334</v>
+        <v>7.033333333333333</v>
       </c>
       <c r="AA255" t="n">
         <v>1</v>
@@ -24117,7 +24117,7 @@
         <v>0.001905724359327946</v>
       </c>
       <c r="Z256" t="n">
-        <v>7.033333333333334</v>
+        <v>7.033333333333333</v>
       </c>
       <c r="AA256" t="n">
         <v>1</v>
@@ -24210,7 +24210,7 @@
         <v>0.001905724359327946</v>
       </c>
       <c r="Z257" t="n">
-        <v>7.033333333333333</v>
+        <v>7.033333333333335</v>
       </c>
       <c r="AA257" t="n">
         <v>1</v>
@@ -24760,7 +24760,7 @@
         <v>0.002926723212164678</v>
       </c>
       <c r="Z263" t="n">
-        <v>5.916666666666666</v>
+        <v>5.916666666666667</v>
       </c>
       <c r="AA263" t="n">
         <v>2</v>
@@ -24938,7 +24938,7 @@
         <v>0.004174246710644446</v>
       </c>
       <c r="Z265" t="n">
-        <v>22.23571428571428</v>
+        <v>22.23571428571429</v>
       </c>
       <c r="AA265" t="n">
         <v>3</v>
@@ -25116,7 +25116,7 @@
         <v>0.006562735571552793</v>
       </c>
       <c r="Z267" t="n">
-        <v>29.21071428571428</v>
+        <v>29.21071428571429</v>
       </c>
       <c r="AA267" t="n">
         <v>5</v>
@@ -25364,7 +25364,7 @@
         <v>0.003529815620086692</v>
       </c>
       <c r="S270" t="n">
-        <v>4.866666666666666</v>
+        <v>4.866666666666667</v>
       </c>
       <c r="T270" t="n">
         <v>2</v>
@@ -25451,7 +25451,7 @@
         <v>0.003529815620086692</v>
       </c>
       <c r="S271" t="n">
-        <v>4.866666666666666</v>
+        <v>4.866666666666667</v>
       </c>
       <c r="T271" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
Alle Files auf lauffhäigkeit überprüft
</commit_message>
<xml_diff>
--- a/transformed_data/cartel_networks/cartel_data_with_centrality_measures.xlsx
+++ b/transformed_data/cartel_networks/cartel_data_with_centrality_measures.xlsx
@@ -657,7 +657,7 @@
         <v>0.006032432325946102</v>
       </c>
       <c r="Z2" t="n">
-        <v>27.3968253968254</v>
+        <v>27.39682539682539</v>
       </c>
       <c r="AA2" t="n">
         <v>5</v>
@@ -750,7 +750,7 @@
         <v>0.003884517316208416</v>
       </c>
       <c r="Z3" t="n">
-        <v>26.67619047619048</v>
+        <v>26.67619047619047</v>
       </c>
       <c r="AA3" t="n">
         <v>3</v>
@@ -843,7 +843,7 @@
         <v>0.00156945221192517</v>
       </c>
       <c r="Z4" t="n">
-        <v>21.63015873015873</v>
+        <v>21.63015873015872</v>
       </c>
       <c r="AA4" t="n">
         <v>1</v>
@@ -1029,7 +1029,7 @@
         <v>0.00156945221192517</v>
       </c>
       <c r="Z6" t="n">
-        <v>21.63015873015873</v>
+        <v>21.63015873015872</v>
       </c>
       <c r="AA6" t="n">
         <v>1</v>
@@ -1122,7 +1122,7 @@
         <v>0.002804333319768834</v>
       </c>
       <c r="Z7" t="n">
-        <v>24.2968253968254</v>
+        <v>24.29682539682539</v>
       </c>
       <c r="AA7" t="n">
         <v>2</v>
@@ -1469,7 +1469,7 @@
         <v>0.00547263705753988</v>
       </c>
       <c r="S11" t="n">
-        <v>21.96349206349205</v>
+        <v>21.96349206349204</v>
       </c>
       <c r="T11" t="n">
         <v>4</v>
@@ -1560,7 +1560,7 @@
         <v>0.00547263705753988</v>
       </c>
       <c r="S12" t="n">
-        <v>21.96349206349205</v>
+        <v>21.96349206349204</v>
       </c>
       <c r="T12" t="n">
         <v>4</v>
@@ -1651,7 +1651,7 @@
         <v>0.00547263705753988</v>
       </c>
       <c r="S13" t="n">
-        <v>21.96349206349205</v>
+        <v>21.96349206349204</v>
       </c>
       <c r="T13" t="n">
         <v>4</v>
@@ -1742,7 +1742,7 @@
         <v>0.00547263705753988</v>
       </c>
       <c r="S14" t="n">
-        <v>21.96349206349205</v>
+        <v>21.96349206349204</v>
       </c>
       <c r="T14" t="n">
         <v>4</v>
@@ -1763,7 +1763,7 @@
         <v>0.006032432325946102</v>
       </c>
       <c r="Z14" t="n">
-        <v>27.3968253968254</v>
+        <v>27.39682539682539</v>
       </c>
       <c r="AA14" t="n">
         <v>5</v>
@@ -2670,7 +2670,7 @@
         <v>0.003224627315347335</v>
       </c>
       <c r="S24" t="n">
-        <v>19.32817460317459</v>
+        <v>19.32817460317458</v>
       </c>
       <c r="T24" t="n">
         <v>2</v>
@@ -2761,7 +2761,7 @@
         <v>0.003224627315347335</v>
       </c>
       <c r="S25" t="n">
-        <v>19.32817460317459</v>
+        <v>19.32817460317458</v>
       </c>
       <c r="T25" t="n">
         <v>2</v>
@@ -3036,7 +3036,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S28" t="n">
-        <v>6.833333333333333</v>
+        <v>6.833333333333334</v>
       </c>
       <c r="T28" t="n">
         <v>5</v>
@@ -3129,7 +3129,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S29" t="n">
-        <v>6.833333333333333</v>
+        <v>6.833333333333334</v>
       </c>
       <c r="T29" t="n">
         <v>5</v>
@@ -3150,7 +3150,7 @@
         <v>0.001952215469372171</v>
       </c>
       <c r="Z29" t="n">
-        <v>4.333333333333333</v>
+        <v>4.333333333333334</v>
       </c>
       <c r="AA29" t="n">
         <v>1</v>
@@ -3222,7 +3222,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S30" t="n">
-        <v>6.833333333333333</v>
+        <v>6.833333333333334</v>
       </c>
       <c r="T30" t="n">
         <v>5</v>
@@ -3243,7 +3243,7 @@
         <v>0.001952215469372171</v>
       </c>
       <c r="Z30" t="n">
-        <v>4.333333333333333</v>
+        <v>4.333333333333334</v>
       </c>
       <c r="AA30" t="n">
         <v>1</v>
@@ -3315,7 +3315,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S31" t="n">
-        <v>6.833333333333333</v>
+        <v>6.833333333333334</v>
       </c>
       <c r="T31" t="n">
         <v>5</v>
@@ -3408,7 +3408,7 @@
         <v>0.008577738442612826</v>
       </c>
       <c r="S32" t="n">
-        <v>6.833333333333333</v>
+        <v>6.833333333333334</v>
       </c>
       <c r="T32" t="n">
         <v>5</v>
@@ -5641,7 +5641,7 @@
         <v>0.001952215469372171</v>
       </c>
       <c r="Z56" t="n">
-        <v>4.333333333333333</v>
+        <v>4.333333333333334</v>
       </c>
       <c r="AA56" t="n">
         <v>1</v>
@@ -5734,7 +5734,7 @@
         <v>0.001952215469372171</v>
       </c>
       <c r="Z57" t="n">
-        <v>4.333333333333333</v>
+        <v>4.333333333333334</v>
       </c>
       <c r="AA57" t="n">
         <v>1</v>
@@ -5827,7 +5827,7 @@
         <v>0.001952215469372171</v>
       </c>
       <c r="Z58" t="n">
-        <v>4.333333333333333</v>
+        <v>4.333333333333334</v>
       </c>
       <c r="AA58" t="n">
         <v>1</v>
@@ -5920,7 +5920,7 @@
         <v>0.001952215469372171</v>
       </c>
       <c r="Z59" t="n">
-        <v>4.333333333333333</v>
+        <v>4.333333333333334</v>
       </c>
       <c r="AA59" t="n">
         <v>1</v>
@@ -5992,7 +5992,7 @@
         <v>0.0104464942771786</v>
       </c>
       <c r="S60" t="n">
-        <v>9.666666666666668</v>
+        <v>9.666666666666666</v>
       </c>
       <c r="T60" t="n">
         <v>7</v>
@@ -6013,7 +6013,7 @@
         <v>0.001762389124862823</v>
       </c>
       <c r="Z60" t="n">
-        <v>5.916666666666667</v>
+        <v>5.916666666666666</v>
       </c>
       <c r="AA60" t="n">
         <v>1</v>
@@ -6085,7 +6085,7 @@
         <v>0.0104464942771786</v>
       </c>
       <c r="S61" t="n">
-        <v>9.666666666666668</v>
+        <v>9.666666666666666</v>
       </c>
       <c r="T61" t="n">
         <v>7</v>
@@ -6106,7 +6106,7 @@
         <v>0.001762389124862823</v>
       </c>
       <c r="Z61" t="n">
-        <v>5.916666666666667</v>
+        <v>5.916666666666666</v>
       </c>
       <c r="AA61" t="n">
         <v>1</v>
@@ -6178,7 +6178,7 @@
         <v>0.0104464942771786</v>
       </c>
       <c r="S62" t="n">
-        <v>9.666666666666668</v>
+        <v>9.666666666666666</v>
       </c>
       <c r="T62" t="n">
         <v>7</v>
@@ -6199,7 +6199,7 @@
         <v>0.00297776980412998</v>
       </c>
       <c r="Z62" t="n">
-        <v>7.583333333333334</v>
+        <v>7.583333333333333</v>
       </c>
       <c r="AA62" t="n">
         <v>2</v>
@@ -6271,7 +6271,7 @@
         <v>0.0104464942771786</v>
       </c>
       <c r="S63" t="n">
-        <v>9.666666666666668</v>
+        <v>9.666666666666666</v>
       </c>
       <c r="T63" t="n">
         <v>7</v>
@@ -6292,7 +6292,7 @@
         <v>0.001762389124862823</v>
       </c>
       <c r="Z63" t="n">
-        <v>5.916666666666667</v>
+        <v>5.916666666666666</v>
       </c>
       <c r="AA63" t="n">
         <v>1</v>
@@ -6364,7 +6364,7 @@
         <v>0.0104464942771786</v>
       </c>
       <c r="S64" t="n">
-        <v>9.666666666666668</v>
+        <v>9.666666666666666</v>
       </c>
       <c r="T64" t="n">
         <v>7</v>
@@ -6385,7 +6385,7 @@
         <v>0.001762389124862823</v>
       </c>
       <c r="Z64" t="n">
-        <v>5.916666666666667</v>
+        <v>5.916666666666666</v>
       </c>
       <c r="AA64" t="n">
         <v>1</v>
@@ -6457,7 +6457,7 @@
         <v>0.0104464942771786</v>
       </c>
       <c r="S65" t="n">
-        <v>9.666666666666668</v>
+        <v>9.666666666666666</v>
       </c>
       <c r="T65" t="n">
         <v>7</v>
@@ -6478,7 +6478,7 @@
         <v>0.001762389124862823</v>
       </c>
       <c r="Z65" t="n">
-        <v>5.916666666666667</v>
+        <v>5.916666666666666</v>
       </c>
       <c r="AA65" t="n">
         <v>1</v>
@@ -6550,7 +6550,7 @@
         <v>0.0104464942771786</v>
       </c>
       <c r="S66" t="n">
-        <v>9.666666666666668</v>
+        <v>9.666666666666666</v>
       </c>
       <c r="T66" t="n">
         <v>7</v>
@@ -6664,7 +6664,7 @@
         <v>0.002867355746022141</v>
       </c>
       <c r="Z67" t="n">
-        <v>18.36785714285713</v>
+        <v>18.36785714285714</v>
       </c>
       <c r="AA67" t="n">
         <v>2</v>
@@ -7288,7 +7288,7 @@
         <v>0.004090150686838246</v>
       </c>
       <c r="S74" t="n">
-        <v>21.64999999999998</v>
+        <v>21.64999999999999</v>
       </c>
       <c r="T74" t="n">
         <v>3</v>
@@ -7309,7 +7309,7 @@
         <v>0.002867355746022141</v>
       </c>
       <c r="Z74" t="n">
-        <v>18.36785714285713</v>
+        <v>18.36785714285714</v>
       </c>
       <c r="AA74" t="n">
         <v>2</v>
@@ -7381,7 +7381,7 @@
         <v>0.004090150686838246</v>
       </c>
       <c r="S75" t="n">
-        <v>21.64999999999998</v>
+        <v>21.64999999999999</v>
       </c>
       <c r="T75" t="n">
         <v>3</v>
@@ -7402,7 +7402,7 @@
         <v>0.004174246710644446</v>
       </c>
       <c r="Z75" t="n">
-        <v>22.23571428571429</v>
+        <v>22.23571428571428</v>
       </c>
       <c r="AA75" t="n">
         <v>3</v>
@@ -7474,7 +7474,7 @@
         <v>0.004090150686838246</v>
       </c>
       <c r="S76" t="n">
-        <v>21.64999999999998</v>
+        <v>21.64999999999999</v>
       </c>
       <c r="T76" t="n">
         <v>3</v>
@@ -7939,7 +7939,7 @@
         <v>0.003756245390724891</v>
       </c>
       <c r="S81" t="n">
-        <v>5.166666666666666</v>
+        <v>5.166666666666667</v>
       </c>
       <c r="T81" t="n">
         <v>2</v>
@@ -8032,7 +8032,7 @@
         <v>0.003756245390724891</v>
       </c>
       <c r="S82" t="n">
-        <v>5.166666666666666</v>
+        <v>5.166666666666667</v>
       </c>
       <c r="T82" t="n">
         <v>2</v>
@@ -8326,7 +8326,7 @@
         <v>0.001655839492786507</v>
       </c>
       <c r="Z85" t="n">
-        <v>20.12023809523809</v>
+        <v>20.12023809523808</v>
       </c>
       <c r="AA85" t="n">
         <v>1</v>
@@ -8508,7 +8508,7 @@
         <v>0.003884517316208416</v>
       </c>
       <c r="Z87" t="n">
-        <v>26.67619047619048</v>
+        <v>26.67619047619047</v>
       </c>
       <c r="AA87" t="n">
         <v>3</v>
@@ -8599,7 +8599,7 @@
         <v>0.001655839492786507</v>
       </c>
       <c r="Z88" t="n">
-        <v>20.12023809523809</v>
+        <v>20.12023809523808</v>
       </c>
       <c r="AA88" t="n">
         <v>1</v>
@@ -8690,7 +8690,7 @@
         <v>0.001655839492786507</v>
       </c>
       <c r="Z89" t="n">
-        <v>20.12023809523809</v>
+        <v>20.12023809523808</v>
       </c>
       <c r="AA89" t="n">
         <v>1</v>
@@ -8781,7 +8781,7 @@
         <v>0.001655839492786507</v>
       </c>
       <c r="Z90" t="n">
-        <v>20.12023809523809</v>
+        <v>20.12023809523808</v>
       </c>
       <c r="AA90" t="n">
         <v>1</v>
@@ -8872,7 +8872,7 @@
         <v>0.001655839492786507</v>
       </c>
       <c r="Z91" t="n">
-        <v>20.12023809523809</v>
+        <v>20.12023809523808</v>
       </c>
       <c r="AA91" t="n">
         <v>1</v>
@@ -8963,7 +8963,7 @@
         <v>0.001655839492786507</v>
       </c>
       <c r="Z92" t="n">
-        <v>20.12023809523809</v>
+        <v>20.12023809523808</v>
       </c>
       <c r="AA92" t="n">
         <v>1</v>
@@ -9126,7 +9126,7 @@
         <v>0.003734692891254172</v>
       </c>
       <c r="S94" t="n">
-        <v>13.37002164502164</v>
+        <v>13.37002164502163</v>
       </c>
       <c r="T94" t="n">
         <v>2</v>
@@ -9147,7 +9147,7 @@
         <v>0.003466064552194036</v>
       </c>
       <c r="Z94" t="n">
-        <v>15.2797619047619</v>
+        <v>15.27976190476189</v>
       </c>
       <c r="AA94" t="n">
         <v>2</v>
@@ -9219,7 +9219,7 @@
         <v>0.003734692891254172</v>
       </c>
       <c r="S95" t="n">
-        <v>13.37002164502164</v>
+        <v>13.37002164502163</v>
       </c>
       <c r="T95" t="n">
         <v>2</v>
@@ -9240,7 +9240,7 @@
         <v>0.002080987983374498</v>
       </c>
       <c r="Z95" t="n">
-        <v>11.3342352092352</v>
+        <v>11.33423520923519</v>
       </c>
       <c r="AA95" t="n">
         <v>1</v>
@@ -9312,7 +9312,7 @@
         <v>0.004066892896957142</v>
       </c>
       <c r="S96" t="n">
-        <v>22.47976190476189</v>
+        <v>22.47976190476188</v>
       </c>
       <c r="T96" t="n">
         <v>3</v>
@@ -9333,7 +9333,7 @@
         <v>0.001646067716759898</v>
       </c>
       <c r="Z96" t="n">
-        <v>17.40039682539682</v>
+        <v>17.40039682539681</v>
       </c>
       <c r="AA96" t="n">
         <v>1</v>
@@ -9405,7 +9405,7 @@
         <v>0.004066892896957142</v>
       </c>
       <c r="S97" t="n">
-        <v>22.47976190476189</v>
+        <v>22.47976190476188</v>
       </c>
       <c r="T97" t="n">
         <v>3</v>
@@ -9426,7 +9426,7 @@
         <v>0.003884517316208416</v>
       </c>
       <c r="Z97" t="n">
-        <v>26.67619047619048</v>
+        <v>26.67619047619047</v>
       </c>
       <c r="AA97" t="n">
         <v>3</v>
@@ -9498,7 +9498,7 @@
         <v>0.004066892896957142</v>
       </c>
       <c r="S98" t="n">
-        <v>22.47976190476189</v>
+        <v>22.47976190476188</v>
       </c>
       <c r="T98" t="n">
         <v>3</v>
@@ -9984,7 +9984,7 @@
         <v>0.00297776980412998</v>
       </c>
       <c r="Z103" t="n">
-        <v>7.583333333333334</v>
+        <v>7.583333333333333</v>
       </c>
       <c r="AA103" t="n">
         <v>2</v>
@@ -10705,7 +10705,7 @@
         <v>0.004846611458008186</v>
       </c>
       <c r="S111" t="n">
-        <v>4.333333333333334</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="T111" t="n">
         <v>3</v>
@@ -10796,7 +10796,7 @@
         <v>0.004846611458008186</v>
       </c>
       <c r="S112" t="n">
-        <v>4.333333333333334</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="T112" t="n">
         <v>3</v>
@@ -10887,7 +10887,7 @@
         <v>0.004846611458008186</v>
       </c>
       <c r="S113" t="n">
-        <v>4.333333333333334</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="T113" t="n">
         <v>3</v>
@@ -11001,7 +11001,7 @@
         <v>0.006032432325946102</v>
       </c>
       <c r="Z114" t="n">
-        <v>27.3968253968254</v>
+        <v>27.39682539682539</v>
       </c>
       <c r="AA114" t="n">
         <v>5</v>
@@ -11555,7 +11555,7 @@
         <v>0.003466064552194036</v>
       </c>
       <c r="Z120" t="n">
-        <v>15.2797619047619</v>
+        <v>15.27976190476189</v>
       </c>
       <c r="AA120" t="n">
         <v>2</v>
@@ -12460,7 +12460,7 @@
         <v>0.00297774247180845</v>
       </c>
       <c r="S130" t="n">
-        <v>4.733333333333334</v>
+        <v>4.733333333333333</v>
       </c>
       <c r="T130" t="n">
         <v>2</v>
@@ -12553,7 +12553,7 @@
         <v>0.00297774247180845</v>
       </c>
       <c r="S131" t="n">
-        <v>4.733333333333334</v>
+        <v>4.733333333333333</v>
       </c>
       <c r="T131" t="n">
         <v>2</v>
@@ -13293,7 +13293,7 @@
         <v>0.004444447588323335</v>
       </c>
       <c r="S139" t="n">
-        <v>6.999999999999999</v>
+        <v>7</v>
       </c>
       <c r="T139" t="n">
         <v>3</v>
@@ -13386,7 +13386,7 @@
         <v>0.004444447588323335</v>
       </c>
       <c r="S140" t="n">
-        <v>6.999999999999999</v>
+        <v>7</v>
       </c>
       <c r="T140" t="n">
         <v>3</v>
@@ -13479,7 +13479,7 @@
         <v>0.004444447588323335</v>
       </c>
       <c r="S141" t="n">
-        <v>6.999999999999999</v>
+        <v>7</v>
       </c>
       <c r="T141" t="n">
         <v>3</v>
@@ -13959,7 +13959,7 @@
         <v>0.004174246710644446</v>
       </c>
       <c r="Z146" t="n">
-        <v>22.23571428571429</v>
+        <v>22.23571428571428</v>
       </c>
       <c r="AA146" t="n">
         <v>3</v>
@@ -14122,7 +14122,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S148" t="n">
-        <v>25.5801587301587</v>
+        <v>25.58015873015871</v>
       </c>
       <c r="T148" t="n">
         <v>9</v>
@@ -14143,7 +14143,7 @@
         <v>0.001728302160475243</v>
       </c>
       <c r="Z148" t="n">
-        <v>18.30241702741702</v>
+        <v>18.30241702741701</v>
       </c>
       <c r="AA148" t="n">
         <v>1</v>
@@ -14213,7 +14213,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S149" t="n">
-        <v>25.5801587301587</v>
+        <v>25.58015873015871</v>
       </c>
       <c r="T149" t="n">
         <v>9</v>
@@ -14234,7 +14234,7 @@
         <v>0.001728302160475243</v>
       </c>
       <c r="Z149" t="n">
-        <v>18.30241702741702</v>
+        <v>18.30241702741701</v>
       </c>
       <c r="AA149" t="n">
         <v>1</v>
@@ -14304,7 +14304,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S150" t="n">
-        <v>25.5801587301587</v>
+        <v>25.58015873015871</v>
       </c>
       <c r="T150" t="n">
         <v>9</v>
@@ -14325,7 +14325,7 @@
         <v>0.001728302160475243</v>
       </c>
       <c r="Z150" t="n">
-        <v>18.30241702741702</v>
+        <v>18.30241702741701</v>
       </c>
       <c r="AA150" t="n">
         <v>1</v>
@@ -14395,7 +14395,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S151" t="n">
-        <v>25.5801587301587</v>
+        <v>25.58015873015871</v>
       </c>
       <c r="T151" t="n">
         <v>9</v>
@@ -14416,7 +14416,7 @@
         <v>0.001728302160475243</v>
       </c>
       <c r="Z151" t="n">
-        <v>18.30241702741702</v>
+        <v>18.30241702741701</v>
       </c>
       <c r="AA151" t="n">
         <v>1</v>
@@ -14486,7 +14486,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S152" t="n">
-        <v>25.5801587301587</v>
+        <v>25.58015873015871</v>
       </c>
       <c r="T152" t="n">
         <v>9</v>
@@ -14507,7 +14507,7 @@
         <v>0.001728302160475243</v>
       </c>
       <c r="Z152" t="n">
-        <v>18.30241702741702</v>
+        <v>18.30241702741701</v>
       </c>
       <c r="AA152" t="n">
         <v>1</v>
@@ -14577,7 +14577,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S153" t="n">
-        <v>25.5801587301587</v>
+        <v>25.58015873015871</v>
       </c>
       <c r="T153" t="n">
         <v>9</v>
@@ -14598,7 +14598,7 @@
         <v>0.001728302160475243</v>
       </c>
       <c r="Z153" t="n">
-        <v>18.30241702741702</v>
+        <v>18.30241702741701</v>
       </c>
       <c r="AA153" t="n">
         <v>1</v>
@@ -14668,7 +14668,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S154" t="n">
-        <v>25.5801587301587</v>
+        <v>25.58015873015871</v>
       </c>
       <c r="T154" t="n">
         <v>9</v>
@@ -14759,7 +14759,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S155" t="n">
-        <v>25.5801587301587</v>
+        <v>25.58015873015871</v>
       </c>
       <c r="T155" t="n">
         <v>9</v>
@@ -14780,7 +14780,7 @@
         <v>0.003903361639413343</v>
       </c>
       <c r="Z155" t="n">
-        <v>23.90039682539683</v>
+        <v>23.90039682539682</v>
       </c>
       <c r="AA155" t="n">
         <v>3</v>
@@ -14850,7 +14850,7 @@
         <v>0.0130712346549076</v>
       </c>
       <c r="S156" t="n">
-        <v>25.5801587301587</v>
+        <v>25.58015873015871</v>
       </c>
       <c r="T156" t="n">
         <v>9</v>
@@ -14871,7 +14871,7 @@
         <v>0.002804333319768834</v>
       </c>
       <c r="Z156" t="n">
-        <v>24.2968253968254</v>
+        <v>24.29682539682539</v>
       </c>
       <c r="AA156" t="n">
         <v>2</v>
@@ -14943,7 +14943,7 @@
         <v>0.007216240904336362</v>
       </c>
       <c r="S157" t="n">
-        <v>27.72976190476189</v>
+        <v>27.72976190476188</v>
       </c>
       <c r="T157" t="n">
         <v>6</v>
@@ -15036,7 +15036,7 @@
         <v>0.007216240904336362</v>
       </c>
       <c r="S158" t="n">
-        <v>27.72976190476189</v>
+        <v>27.72976190476188</v>
       </c>
       <c r="T158" t="n">
         <v>6</v>
@@ -15129,7 +15129,7 @@
         <v>0.007216240904336362</v>
       </c>
       <c r="S159" t="n">
-        <v>27.72976190476189</v>
+        <v>27.72976190476188</v>
       </c>
       <c r="T159" t="n">
         <v>6</v>
@@ -15150,7 +15150,7 @@
         <v>0.006032432325946102</v>
       </c>
       <c r="Z159" t="n">
-        <v>27.3968253968254</v>
+        <v>27.39682539682539</v>
       </c>
       <c r="AA159" t="n">
         <v>5</v>
@@ -15222,7 +15222,7 @@
         <v>0.007216240904336362</v>
       </c>
       <c r="S160" t="n">
-        <v>27.72976190476189</v>
+        <v>27.72976190476188</v>
       </c>
       <c r="T160" t="n">
         <v>6</v>
@@ -15315,7 +15315,7 @@
         <v>0.007216240904336362</v>
       </c>
       <c r="S161" t="n">
-        <v>27.72976190476189</v>
+        <v>27.72976190476188</v>
       </c>
       <c r="T161" t="n">
         <v>6</v>
@@ -15336,7 +15336,7 @@
         <v>0.003903361639413343</v>
       </c>
       <c r="Z161" t="n">
-        <v>23.90039682539683</v>
+        <v>23.90039682539682</v>
       </c>
       <c r="AA161" t="n">
         <v>3</v>
@@ -15408,7 +15408,7 @@
         <v>0.007216240904336362</v>
       </c>
       <c r="S162" t="n">
-        <v>27.72976190476189</v>
+        <v>27.72976190476188</v>
       </c>
       <c r="T162" t="n">
         <v>6</v>
@@ -15522,7 +15522,7 @@
         <v>0.001645815673832132</v>
       </c>
       <c r="Z163" t="n">
-        <v>17.56908369408369</v>
+        <v>17.56908369408368</v>
       </c>
       <c r="AA163" t="n">
         <v>1</v>
@@ -15615,7 +15615,7 @@
         <v>0.006032432325946102</v>
       </c>
       <c r="Z164" t="n">
-        <v>27.3968253968254</v>
+        <v>27.39682539682539</v>
       </c>
       <c r="AA164" t="n">
         <v>5</v>
@@ -15708,7 +15708,7 @@
         <v>0.003903361639413343</v>
       </c>
       <c r="Z165" t="n">
-        <v>23.90039682539683</v>
+        <v>23.90039682539682</v>
       </c>
       <c r="AA165" t="n">
         <v>3</v>
@@ -15801,7 +15801,7 @@
         <v>0.001645815673832132</v>
       </c>
       <c r="Z166" t="n">
-        <v>17.56908369408369</v>
+        <v>17.56908369408368</v>
       </c>
       <c r="AA166" t="n">
         <v>1</v>
@@ -15871,7 +15871,7 @@
         <v>0.001608707494018752</v>
       </c>
       <c r="S167" t="n">
-        <v>21.05396825396825</v>
+        <v>21.05396825396824</v>
       </c>
       <c r="T167" t="n">
         <v>1</v>
@@ -17742,7 +17742,7 @@
         <v>0.001913327899506806</v>
       </c>
       <c r="Z187" t="n">
-        <v>14.57150072150072</v>
+        <v>14.57150072150071</v>
       </c>
       <c r="AA187" t="n">
         <v>1</v>
@@ -17835,7 +17835,7 @@
         <v>0.003184124331344304</v>
       </c>
       <c r="Z188" t="n">
-        <v>20.72698412698413</v>
+        <v>20.72698412698412</v>
       </c>
       <c r="AA188" t="n">
         <v>2</v>
@@ -17928,7 +17928,7 @@
         <v>0.001913327899506806</v>
       </c>
       <c r="Z189" t="n">
-        <v>14.57150072150072</v>
+        <v>14.57150072150071</v>
       </c>
       <c r="AA189" t="n">
         <v>1</v>
@@ -18021,7 +18021,7 @@
         <v>0.001913327899506806</v>
       </c>
       <c r="Z190" t="n">
-        <v>14.57150072150072</v>
+        <v>14.57150072150071</v>
       </c>
       <c r="AA190" t="n">
         <v>1</v>
@@ -18114,7 +18114,7 @@
         <v>0.001913327899506806</v>
       </c>
       <c r="Z191" t="n">
-        <v>14.57150072150072</v>
+        <v>14.57150072150071</v>
       </c>
       <c r="AA191" t="n">
         <v>1</v>
@@ -18573,7 +18573,7 @@
         <v>0.001701332547968635</v>
       </c>
       <c r="Z196" t="n">
-        <v>18.31031746031746</v>
+        <v>18.31031746031745</v>
       </c>
       <c r="AA196" t="n">
         <v>1</v>
@@ -19503,7 +19503,7 @@
         <v>0.001764217484469077</v>
       </c>
       <c r="Z206" t="n">
-        <v>19.06031746031746</v>
+        <v>19.06031746031745</v>
       </c>
       <c r="AA206" t="n">
         <v>1</v>
@@ -19596,7 +19596,7 @@
         <v>0.001764217484469077</v>
       </c>
       <c r="Z207" t="n">
-        <v>19.06031746031746</v>
+        <v>19.06031746031745</v>
       </c>
       <c r="AA207" t="n">
         <v>1</v>
@@ -19689,7 +19689,7 @@
         <v>0.003184124331344304</v>
       </c>
       <c r="Z208" t="n">
-        <v>20.72698412698413</v>
+        <v>20.72698412698412</v>
       </c>
       <c r="AA208" t="n">
         <v>2</v>
@@ -19782,7 +19782,7 @@
         <v>0.001764217484469077</v>
       </c>
       <c r="Z209" t="n">
-        <v>19.06031746031746</v>
+        <v>19.06031746031745</v>
       </c>
       <c r="AA209" t="n">
         <v>1</v>
@@ -19968,7 +19968,7 @@
         <v>0.001764217484469077</v>
       </c>
       <c r="Z211" t="n">
-        <v>19.06031746031746</v>
+        <v>19.06031746031745</v>
       </c>
       <c r="AA211" t="n">
         <v>1</v>
@@ -20061,7 +20061,7 @@
         <v>0.001764217484469077</v>
       </c>
       <c r="Z212" t="n">
-        <v>19.06031746031746</v>
+        <v>19.06031746031745</v>
       </c>
       <c r="AA212" t="n">
         <v>1</v>
@@ -20154,7 +20154,7 @@
         <v>0.001764217484469077</v>
       </c>
       <c r="Z213" t="n">
-        <v>19.06031746031746</v>
+        <v>19.06031746031745</v>
       </c>
       <c r="AA213" t="n">
         <v>1</v>
@@ -20983,7 +20983,7 @@
         <v>0.001890394166277293</v>
       </c>
       <c r="Z222" t="n">
-        <v>7.366666666666666</v>
+        <v>7.366666666666668</v>
       </c>
       <c r="AA222" t="n">
         <v>1</v>
@@ -21074,7 +21074,7 @@
         <v>0.001890394166277293</v>
       </c>
       <c r="Z223" t="n">
-        <v>7.366666666666666</v>
+        <v>7.366666666666668</v>
       </c>
       <c r="AA223" t="n">
         <v>1</v>
@@ -21165,7 +21165,7 @@
         <v>0.001890394166277293</v>
       </c>
       <c r="Z224" t="n">
-        <v>7.366666666666666</v>
+        <v>7.366666666666668</v>
       </c>
       <c r="AA224" t="n">
         <v>1</v>
@@ -21256,7 +21256,7 @@
         <v>0.001890394166277293</v>
       </c>
       <c r="Z225" t="n">
-        <v>7.366666666666666</v>
+        <v>7.366666666666668</v>
       </c>
       <c r="AA225" t="n">
         <v>1</v>
@@ -21347,7 +21347,7 @@
         <v>0.001890394166277293</v>
       </c>
       <c r="Z226" t="n">
-        <v>7.366666666666666</v>
+        <v>7.366666666666668</v>
       </c>
       <c r="AA226" t="n">
         <v>1</v>
@@ -21438,7 +21438,7 @@
         <v>0.001890394166277293</v>
       </c>
       <c r="Z227" t="n">
-        <v>7.366666666666666</v>
+        <v>7.366666666666668</v>
       </c>
       <c r="AA227" t="n">
         <v>1</v>
@@ -21601,7 +21601,7 @@
         <v>0.006230585784312563</v>
       </c>
       <c r="S229" t="n">
-        <v>5.666666666666666</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="T229" t="n">
         <v>4</v>
@@ -21694,7 +21694,7 @@
         <v>0.006230585784312563</v>
       </c>
       <c r="S230" t="n">
-        <v>5.666666666666666</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="T230" t="n">
         <v>4</v>
@@ -21787,7 +21787,7 @@
         <v>0.006230585784312563</v>
       </c>
       <c r="S231" t="n">
-        <v>5.666666666666666</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="T231" t="n">
         <v>4</v>
@@ -21880,7 +21880,7 @@
         <v>0.006230585784312563</v>
       </c>
       <c r="S232" t="n">
-        <v>5.666666666666666</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="T232" t="n">
         <v>4</v>
@@ -24210,7 +24210,7 @@
         <v>0.001905724359327946</v>
       </c>
       <c r="Z257" t="n">
-        <v>7.033333333333335</v>
+        <v>7.033333333333333</v>
       </c>
       <c r="AA257" t="n">
         <v>1</v>
@@ -24650,7 +24650,7 @@
         <v>0.004478590456557669</v>
       </c>
       <c r="S262" t="n">
-        <v>5.533333333333333</v>
+        <v>5.533333333333332</v>
       </c>
       <c r="T262" t="n">
         <v>3</v>
@@ -24739,7 +24739,7 @@
         <v>0.004478590456557669</v>
       </c>
       <c r="S263" t="n">
-        <v>5.533333333333333</v>
+        <v>5.533333333333332</v>
       </c>
       <c r="T263" t="n">
         <v>3</v>
@@ -24828,7 +24828,7 @@
         <v>0.004478590456557669</v>
       </c>
       <c r="S264" t="n">
-        <v>5.533333333333333</v>
+        <v>5.533333333333332</v>
       </c>
       <c r="T264" t="n">
         <v>3</v>
@@ -24938,7 +24938,7 @@
         <v>0.004174246710644446</v>
       </c>
       <c r="Z265" t="n">
-        <v>22.23571428571429</v>
+        <v>22.23571428571428</v>
       </c>
       <c r="AA265" t="n">
         <v>3</v>

</xml_diff>